<commit_message>
Added a VB code to resize image to 366 x 366 to mactch standards of gemma3:12B Fixing minor bugs Add a like rescent post if the action is message only added a feature that when initilizing applications it will delete all files in Instgram Images Directory
</commit_message>
<xml_diff>
--- a/InstgramOutput.xlsx
+++ b/InstgramOutput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mehmoud project 3\Instagram-Facebook-Outreaching-Automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LLM VISION Uipath3\LLM VISION Uipath3 Github\Instagram-Facebook-Outreaching-Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5042ADEF-3590-4A7B-907E-F0A7581B9241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A65408-5F7B-4373-ADAB-864A29F264A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11325" xr2:uid="{CB2CBD43-8825-4C50-9713-C3E6C0B6D132}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CB2CBD43-8825-4C50-9713-C3E6C0B6D132}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="78">
   <si>
     <t>https://www.instagram.com/maxwellmcomie</t>
   </si>
@@ -291,6 +291,12 @@
   </si>
   <si>
     <t>Hey Duckie, I love your passion for animals and your commitment to making a difference. As a video editor, I'd be thrilled to help you create powerful content that showcases your work and inspires others to get involved. Let's chat about how we can bring your vision to life!</t>
+  </si>
+  <si>
+    <t>Such a sweet, genuine moment! Capturing these fleeting connections is everything. Do you ever find it challenging to balance documenting &amp; being present? Just sent you something in DMs you might find interesting - check it when you get a chance!</t>
+  </si>
+  <si>
+    <t>Hey! Just saw your video about the new Supra – awesome content! I'm a big car enthusiast myself and really enjoyed your breakdown of the specs. I actually do some editing and motion graphics for a few YouTube channels in the tech space, helping them level up their visuals.I recently helped a channel jump from 2k to 10k subscribers, mostly by refining their video structure and adding some dynamic transitions. I’m Visuals, by the way. Happy to chat about your content if you're ever looking for a fresh perspective!</t>
   </si>
 </sst>
 </file>
@@ -349,9 +355,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -389,7 +395,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -495,7 +501,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -637,7 +643,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -645,7 +651,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAE2015-94EE-4CD3-8429-8AD466D06123}">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1687,6 +1693,29 @@
         <v>0</v>
       </c>
     </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" t="s">
+        <v>76</v>
+      </c>
+      <c r="E57" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" t="b">
+        <v>1</v>
+      </c>
+      <c r="G57" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed argument for Commenting
</commit_message>
<xml_diff>
--- a/InstgramOutput.xlsx
+++ b/InstgramOutput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LLM VISION Uipath3\LLM VISION Uipath3 Github\Instagram-Facebook-Outreaching-Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F885D52-652A-4AF5-AAF5-ED9575680EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F8FC11-4980-4E51-9A4F-21E818E4EF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CB2CBD43-8825-4C50-9713-C3E6C0B6D132}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="130">
   <si>
     <t>Profile url</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>Hey! Just stumbled across your video on [Video Topic] - really enjoyed your style and how you explained things! I've been helping other creators level up their videos recently, even helped someone go from 2K to 10K subscribers. I’m Visuals, I edit for AI and developer channels, and I've got a few growth hacks that could be a good fit for your content. Would you be open to a quick 15-minute chat sometime?</t>
+  </si>
+  <si>
+    <t>This is seriously impressive! The way you handle light &amp; shadow is masterful. Wondering what your go-to brushes are for texture? Just sent you something in DMs you might find interesting - check it when you get a chance!</t>
+  </si>
+  <si>
+    <t>Love the way you play with light and shadow! Really creates a mood. What's your favorite lens for these shots? Just sent you something in DMs you might find interesting - check it when you get a chance!</t>
   </si>
 </sst>
 </file>
@@ -760,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAE2015-94EE-4CD3-8429-8AD466D06123}">
-  <dimension ref="A1:G88"/>
+  <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2585,6 +2591,114 @@
         <v>0</v>
       </c>
     </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>15</v>
+      </c>
+      <c r="B89" t="s">
+        <v>16</v>
+      </c>
+      <c r="C89" t="s">
+        <v>17</v>
+      </c>
+      <c r="D89" t="s">
+        <v>17</v>
+      </c>
+      <c r="E89" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>15</v>
+      </c>
+      <c r="B90" t="s">
+        <v>16</v>
+      </c>
+      <c r="C90" t="b">
+        <v>0</v>
+      </c>
+      <c r="F90" t="b">
+        <v>0</v>
+      </c>
+      <c r="G90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>18</v>
+      </c>
+      <c r="B91" t="s">
+        <v>19</v>
+      </c>
+      <c r="C91" t="b">
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>128</v>
+      </c>
+      <c r="F91" t="b">
+        <v>0</v>
+      </c>
+      <c r="G91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>22</v>
+      </c>
+      <c r="B92" t="s">
+        <v>23</v>
+      </c>
+      <c r="C92" t="b">
+        <v>1</v>
+      </c>
+      <c r="D92" t="s">
+        <v>129</v>
+      </c>
+      <c r="F92" t="b">
+        <v>0</v>
+      </c>
+      <c r="G92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>15</v>
+      </c>
+      <c r="B93" t="s">
+        <v>16</v>
+      </c>
+      <c r="C93" t="s">
+        <v>17</v>
+      </c>
+      <c r="D93" t="s">
+        <v>17</v>
+      </c>
+      <c r="E93" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>15</v>
+      </c>
+      <c r="B94" t="s">
+        <v>16</v>
+      </c>
+      <c r="C94" t="b">
+        <v>0</v>
+      </c>
+      <c r="F94" t="b">
+        <v>0</v>
+      </c>
+      <c r="G94" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix, New feature #6
</commit_message>
<xml_diff>
--- a/InstgramOutput.xlsx
+++ b/InstgramOutput.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Instagram rpa bot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LLM VISION Uipath3\LLM VISION Uipath3 Github\Instagram-Facebook-Outreaching-Automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC4BA3C-ACD1-41AB-9954-9B73D4CCF8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D6914EF-F328-4210-9188-DAA72C791EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CB2CBD43-8825-4C50-9713-C3E6C0B6D132}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CB2CBD43-8825-4C50-9713-C3E6C0B6D132}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="376">
   <si>
     <t>Profile url</t>
   </si>
@@ -1150,6 +1150,9 @@
   </si>
   <si>
     <t>Krystal Rehorn (Robertson)</t>
+  </si>
+  <si>
+    <t>Default</t>
   </si>
 </sst>
 </file>
@@ -1237,9 +1240,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1277,7 +1280,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1383,7 +1386,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1525,7 +1528,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1533,7 +1536,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAE2015-94EE-4CD3-8429-8AD466D06123}">
-  <dimension ref="A1:G171"/>
+  <dimension ref="A1:H179"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="J192" sqref="J192"/>
@@ -4799,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>351</v>
       </c>
@@ -4819,7 +4822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>354</v>
       </c>
@@ -4839,7 +4842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>357</v>
       </c>
@@ -4856,7 +4859,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>357</v>
       </c>
@@ -4876,7 +4879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>359</v>
       </c>
@@ -4896,7 +4899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>362</v>
       </c>
@@ -4916,7 +4919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>365</v>
       </c>
@@ -4933,7 +4936,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>365</v>
       </c>
@@ -4953,7 +4956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>367</v>
       </c>
@@ -4973,7 +4976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>370</v>
       </c>
@@ -4993,7 +4996,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>373</v>
       </c>
@@ -5011,6 +5014,154 @@
       </c>
       <c r="G171" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>246</v>
+      </c>
+      <c r="B172" t="s">
+        <v>247</v>
+      </c>
+      <c r="C172" t="s">
+        <v>9</v>
+      </c>
+      <c r="D172" t="s">
+        <v>9</v>
+      </c>
+      <c r="E172" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>246</v>
+      </c>
+      <c r="B173" t="s">
+        <v>247</v>
+      </c>
+      <c r="C173" t="b">
+        <v>0</v>
+      </c>
+      <c r="F173" t="b">
+        <v>0</v>
+      </c>
+      <c r="G173" t="b">
+        <v>0</v>
+      </c>
+      <c r="H173" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>246</v>
+      </c>
+      <c r="B174" t="s">
+        <v>247</v>
+      </c>
+      <c r="C174" t="s">
+        <v>9</v>
+      </c>
+      <c r="D174" t="s">
+        <v>9</v>
+      </c>
+      <c r="E174" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>246</v>
+      </c>
+      <c r="B175" t="s">
+        <v>247</v>
+      </c>
+      <c r="C175" t="b">
+        <v>0</v>
+      </c>
+      <c r="F175" t="b">
+        <v>0</v>
+      </c>
+      <c r="G175" t="b">
+        <v>0</v>
+      </c>
+      <c r="H175" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>246</v>
+      </c>
+      <c r="B176" t="s">
+        <v>247</v>
+      </c>
+      <c r="C176" t="s">
+        <v>9</v>
+      </c>
+      <c r="D176" t="s">
+        <v>9</v>
+      </c>
+      <c r="E176" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>246</v>
+      </c>
+      <c r="B177" t="s">
+        <v>247</v>
+      </c>
+      <c r="C177" t="b">
+        <v>0</v>
+      </c>
+      <c r="F177" t="b">
+        <v>0</v>
+      </c>
+      <c r="G177" t="b">
+        <v>0</v>
+      </c>
+      <c r="H177" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>246</v>
+      </c>
+      <c r="B178" t="s">
+        <v>247</v>
+      </c>
+      <c r="C178" t="s">
+        <v>9</v>
+      </c>
+      <c r="D178" t="s">
+        <v>9</v>
+      </c>
+      <c r="E178" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>246</v>
+      </c>
+      <c r="B179" t="s">
+        <v>247</v>
+      </c>
+      <c r="C179" t="b">
+        <v>0</v>
+      </c>
+      <c r="F179" t="b">
+        <v>0</v>
+      </c>
+      <c r="G179" t="b">
+        <v>0</v>
+      </c>
+      <c r="H179" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>